<commit_message>
2021/4/2 gyoumu.py get_sorting のsortのアルゴリズムを変更した
</commit_message>
<xml_diff>
--- a/Program/出荷実績照会_本社.xlsx
+++ b/Program/出荷実績照会_本社.xlsx
@@ -8,9 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="新潟運輸_通常_輸出N" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="トール_曜日違い_輸出N" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="新潟運輸_通常_輸出Y" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -176,66 +174,6 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>7</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2400300" cy="595312"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>7</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2400300" cy="595312"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -535,12 +473,12 @@
   <cols>
     <col width="2.42" customWidth="1" min="1" max="1"/>
     <col width="9.350000000000001" customWidth="1" min="2" max="2"/>
-    <col width="13.64" customWidth="1" min="3" max="3"/>
-    <col width="20.57" customWidth="1" min="4" max="4"/>
+    <col width="14.3" customWidth="1" min="3" max="3"/>
+    <col width="26.18" customWidth="1" min="4" max="4"/>
     <col width="10.45" customWidth="1" min="5" max="5"/>
     <col width="8.030000000000001" customWidth="1" min="6" max="6"/>
     <col width="4.29" customWidth="1" min="7" max="7"/>
-    <col width="8.25" customWidth="1" min="8" max="8"/>
+    <col width="9.350000000000001" customWidth="1" min="8" max="8"/>
     <col width="4.29" customWidth="1" min="9" max="9"/>
     <col width="8.030000000000001" customWidth="1" min="10" max="10"/>
     <col width="1.65" customWidth="1" min="11" max="11"/>
@@ -636,39 +574,39 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>20210401</t>
+          <t>20210402</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>タキ倉庫　榛南</t>
+          <t>ｻｶｯｸ㈱本社工場</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>ＰＲ－Ａ(改） (15KG)</t>
+          <t>ＳＴＭ-４０-Ｔ２塗料 (1KG)</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>21032206H</t>
+          <t>21032406H</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>KG</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr">
         <is>
-          <t>T544A27</t>
+          <t>K7322908</t>
         </is>
       </c>
       <c r="I5" s="1" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
@@ -688,396 +626,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:L5"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="2.42" customWidth="1" min="1" max="1"/>
-    <col width="9.350000000000001" customWidth="1" min="2" max="2"/>
-    <col width="9.9" customWidth="1" min="3" max="3"/>
-    <col width="20.24" customWidth="1" min="4" max="4"/>
-    <col width="10.45" customWidth="1" min="5" max="5"/>
-    <col width="8.030000000000001" customWidth="1" min="6" max="6"/>
-    <col width="4.29" customWidth="1" min="7" max="7"/>
-    <col width="7.590000000000001" customWidth="1" min="8" max="8"/>
-    <col width="4.29" customWidth="1" min="9" max="9"/>
-    <col width="8.030000000000001" customWidth="1" min="10" max="10"/>
-    <col width="1.65" customWidth="1" min="11" max="11"/>
-    <col width="3.850000000000001" customWidth="1" min="12" max="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="23" customHeight="1">
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>出荷実績照会</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="18" customHeight="1">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>出荷工場：@0001 本社工場</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="18" customHeight="1">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>運送業者：U0001 トール   配送区分：4 曜日違い  輸出：N</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="18" customHeight="1">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>行</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>売上日</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>納入先名</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>品名</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>ﾛｯﾄNo.</t>
-        </is>
-      </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>売上数量</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>単位</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>注文No.</t>
-        </is>
-      </c>
-      <c r="I4" s="1" t="inlineStr">
-        <is>
-          <t>缶数</t>
-        </is>
-      </c>
-      <c r="J4" s="1" t="inlineStr">
-        <is>
-          <t>備考</t>
-        </is>
-      </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="L4" s="1" t="inlineStr">
-        <is>
-          <t>add</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="18" customHeight="1">
-      <c r="A5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>20210401</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>白水ＤＨＣ</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>ＳＴＭ－１塗料 (1KG)</t>
-        </is>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>21021701H</t>
-        </is>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="inlineStr"/>
-      <c r="I5" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="J5" s="1" t="inlineStr">
-        <is>
-          <t>本社出荷</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr"/>
-      <c r="L5" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.2" right="0.2" top="0.8" bottom="0.8" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" paperSize="9" fitToHeight="0" fitToWidth="1"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:L6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="2.42" customWidth="1" min="1" max="1"/>
-    <col width="9.350000000000001" customWidth="1" min="2" max="2"/>
-    <col width="13.64" customWidth="1" min="3" max="3"/>
-    <col width="36.95999999999999" customWidth="1" min="4" max="4"/>
-    <col width="12.65" customWidth="1" min="5" max="5"/>
-    <col width="8.030000000000001" customWidth="1" min="6" max="6"/>
-    <col width="4.29" customWidth="1" min="7" max="7"/>
-    <col width="8.25" customWidth="1" min="8" max="8"/>
-    <col width="4.29" customWidth="1" min="9" max="9"/>
-    <col width="8.030000000000001" customWidth="1" min="10" max="10"/>
-    <col width="1.65" customWidth="1" min="11" max="11"/>
-    <col width="3.850000000000001" customWidth="1" min="12" max="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="23" customHeight="1">
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>出荷実績照会</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="18" customHeight="1">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>出荷工場：@0001 本社工場</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="18" customHeight="1">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>運送業者：U0009 新潟運輸   配送区分：1 通常  輸出：Y</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="18" customHeight="1">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>行</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>売上日</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>納入先名</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>品名</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>ﾛｯﾄNo.</t>
-        </is>
-      </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>売上数量</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>単位</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>注文No.</t>
-        </is>
-      </c>
-      <c r="I4" s="1" t="inlineStr">
-        <is>
-          <t>缶数</t>
-        </is>
-      </c>
-      <c r="J4" s="1" t="inlineStr">
-        <is>
-          <t>備考</t>
-        </is>
-      </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="L4" s="1" t="inlineStr">
-        <is>
-          <t>add</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="18" customHeight="1">
-      <c r="A5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>20210401</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>築港横浜　第２</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>ＳＴＭ－３０－Ｔ２ クリヤー (UN/15KG)</t>
-        </is>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>21030405H</t>
-        </is>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="inlineStr">
-        <is>
-          <t>FG10111</t>
-        </is>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1" t="inlineStr">
-        <is>
-          <t>本社出荷</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="L5" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" ht="18" customHeight="1">
-      <c r="A6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>20210401</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>築港横浜　第２</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="inlineStr">
-        <is>
-          <t>ＳＴＭ－１塗料 (UN/15KG)</t>
-        </is>
-      </c>
-      <c r="E6" s="1" t="inlineStr">
-        <is>
-          <t>21021707H01</t>
-        </is>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="H6" s="1" t="inlineStr">
-        <is>
-          <t>FG10111</t>
-        </is>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1" t="inlineStr">
-        <is>
-          <t>本社出荷</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="L6" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.2" right="0.2" top="0.8" bottom="0.8" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" paperSize="9" fitToHeight="0" fitToWidth="1"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>